<commit_message>
added documentation as word, pdf, and README
</commit_message>
<xml_diff>
--- a/data/gas_prices copy.xlsx
+++ b/data/gas_prices copy.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K309"/>
+  <dimension ref="A1:K389"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13629,10 +13629,8 @@
       <c r="K289" t="inlineStr"/>
     </row>
     <row r="290">
-      <c r="A290" t="inlineStr">
-        <is>
-          <t>65515</t>
-        </is>
+      <c r="A290" t="n">
+        <v>65515</v>
       </c>
       <c r="B290" t="inlineStr">
         <is>
@@ -13674,10 +13672,8 @@
       <c r="K290" t="inlineStr"/>
     </row>
     <row r="291">
-      <c r="A291" t="inlineStr">
-        <is>
-          <t>77205</t>
-        </is>
+      <c r="A291" t="n">
+        <v>77205</v>
       </c>
       <c r="B291" t="inlineStr">
         <is>
@@ -13719,10 +13715,8 @@
       <c r="K291" t="inlineStr"/>
     </row>
     <row r="292">
-      <c r="A292" t="inlineStr">
-        <is>
-          <t>77223</t>
-        </is>
+      <c r="A292" t="n">
+        <v>77223</v>
       </c>
       <c r="B292" t="inlineStr">
         <is>
@@ -13764,10 +13758,8 @@
       <c r="K292" t="inlineStr"/>
     </row>
     <row r="293">
-      <c r="A293" t="inlineStr">
-        <is>
-          <t>65514</t>
-        </is>
+      <c r="A293" t="n">
+        <v>65514</v>
       </c>
       <c r="B293" t="inlineStr">
         <is>
@@ -13809,10 +13801,8 @@
       <c r="K293" t="inlineStr"/>
     </row>
     <row r="294">
-      <c r="A294" t="inlineStr">
-        <is>
-          <t>77232</t>
-        </is>
+      <c r="A294" t="n">
+        <v>77232</v>
       </c>
       <c r="B294" t="inlineStr">
         <is>
@@ -13854,10 +13844,8 @@
       <c r="K294" t="inlineStr"/>
     </row>
     <row r="295">
-      <c r="A295" t="inlineStr">
-        <is>
-          <t>77202</t>
-        </is>
+      <c r="A295" t="n">
+        <v>77202</v>
       </c>
       <c r="B295" t="inlineStr">
         <is>
@@ -13899,10 +13887,8 @@
       <c r="K295" t="inlineStr"/>
     </row>
     <row r="296">
-      <c r="A296" t="inlineStr">
-        <is>
-          <t>86650</t>
-        </is>
+      <c r="A296" t="n">
+        <v>86650</v>
       </c>
       <c r="B296" t="inlineStr">
         <is>
@@ -13944,10 +13930,8 @@
       <c r="K296" t="inlineStr"/>
     </row>
     <row r="297">
-      <c r="A297" t="inlineStr">
-        <is>
-          <t>77218</t>
-        </is>
+      <c r="A297" t="n">
+        <v>77218</v>
       </c>
       <c r="B297" t="inlineStr">
         <is>
@@ -13989,10 +13973,8 @@
       <c r="K297" t="inlineStr"/>
     </row>
     <row r="298">
-      <c r="A298" t="inlineStr">
-        <is>
-          <t>77243</t>
-        </is>
+      <c r="A298" t="n">
+        <v>77243</v>
       </c>
       <c r="B298" t="inlineStr">
         <is>
@@ -14034,10 +14016,8 @@
       <c r="K298" t="inlineStr"/>
     </row>
     <row r="299">
-      <c r="A299" t="inlineStr">
-        <is>
-          <t>77235</t>
-        </is>
+      <c r="A299" t="n">
+        <v>77235</v>
       </c>
       <c r="B299" t="inlineStr">
         <is>
@@ -14079,10 +14059,8 @@
       <c r="K299" t="inlineStr"/>
     </row>
     <row r="300">
-      <c r="A300" t="inlineStr">
-        <is>
-          <t>77228</t>
-        </is>
+      <c r="A300" t="n">
+        <v>77228</v>
       </c>
       <c r="B300" t="inlineStr">
         <is>
@@ -14124,10 +14102,8 @@
       <c r="K300" t="inlineStr"/>
     </row>
     <row r="301">
-      <c r="A301" t="inlineStr">
-        <is>
-          <t>69163</t>
-        </is>
+      <c r="A301" t="n">
+        <v>69163</v>
       </c>
       <c r="B301" t="inlineStr">
         <is>
@@ -14169,10 +14145,8 @@
       <c r="K301" t="inlineStr"/>
     </row>
     <row r="302">
-      <c r="A302" t="inlineStr">
-        <is>
-          <t>109205</t>
-        </is>
+      <c r="A302" t="n">
+        <v>109205</v>
       </c>
       <c r="B302" t="inlineStr">
         <is>
@@ -14214,10 +14188,8 @@
       <c r="K302" t="inlineStr"/>
     </row>
     <row r="303">
-      <c r="A303" t="inlineStr">
-        <is>
-          <t>65512</t>
-        </is>
+      <c r="A303" t="n">
+        <v>65512</v>
       </c>
       <c r="B303" t="inlineStr">
         <is>
@@ -14259,10 +14231,8 @@
       <c r="K303" t="inlineStr"/>
     </row>
     <row r="304">
-      <c r="A304" t="inlineStr">
-        <is>
-          <t>83384</t>
-        </is>
+      <c r="A304" t="n">
+        <v>83384</v>
       </c>
       <c r="B304" t="inlineStr">
         <is>
@@ -14304,10 +14274,8 @@
       <c r="K304" t="inlineStr"/>
     </row>
     <row r="305">
-      <c r="A305" t="inlineStr">
-        <is>
-          <t>77015</t>
-        </is>
+      <c r="A305" t="n">
+        <v>77015</v>
       </c>
       <c r="B305" t="inlineStr">
         <is>
@@ -14349,10 +14317,8 @@
       <c r="K305" t="inlineStr"/>
     </row>
     <row r="306">
-      <c r="A306" t="inlineStr">
-        <is>
-          <t>107728</t>
-        </is>
+      <c r="A306" t="n">
+        <v>107728</v>
       </c>
       <c r="B306" t="inlineStr">
         <is>
@@ -14394,10 +14360,8 @@
       <c r="K306" t="inlineStr"/>
     </row>
     <row r="307">
-      <c r="A307" t="inlineStr">
-        <is>
-          <t>65572</t>
-        </is>
+      <c r="A307" t="n">
+        <v>65572</v>
       </c>
       <c r="B307" t="inlineStr">
         <is>
@@ -14439,10 +14403,8 @@
       <c r="K307" t="inlineStr"/>
     </row>
     <row r="308">
-      <c r="A308" t="inlineStr">
-        <is>
-          <t>65511</t>
-        </is>
+      <c r="A308" t="n">
+        <v>65511</v>
       </c>
       <c r="B308" t="inlineStr">
         <is>
@@ -14484,10 +14446,8 @@
       <c r="K308" t="inlineStr"/>
     </row>
     <row r="309">
-      <c r="A309" t="inlineStr">
-        <is>
-          <t>65556</t>
-        </is>
+      <c r="A309" t="n">
+        <v>65556</v>
       </c>
       <c r="B309" t="inlineStr">
         <is>
@@ -14527,6 +14487,3438 @@
       </c>
       <c r="J309" t="inlineStr"/>
       <c r="K309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>65542</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>3250 MacDonald St</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2573819, 'Longitude': -123.1680407}</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>2025-06-01T09:14:50.302Z</t>
+        </is>
+      </c>
+      <c r="G310" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H310" t="inlineStr"/>
+      <c r="I310" t="inlineStr"/>
+      <c r="J310" t="inlineStr"/>
+      <c r="K310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>65533</v>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>4615 Arbutus St</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2449719, 'Longitude': -123.1540385}</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>2025-06-01T02:10:53.532Z</t>
+        </is>
+      </c>
+      <c r="G311" t="n">
+        <v>160.9</v>
+      </c>
+      <c r="H311" t="inlineStr">
+        <is>
+          <t>2025-06-01T02:10:53.563Z</t>
+        </is>
+      </c>
+      <c r="I311" t="n">
+        <v>185.9</v>
+      </c>
+      <c r="J311" t="inlineStr"/>
+      <c r="K311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>83068</v>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>3205 Arbutus St</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.256927568207, 'Longitude': -123.153288960457}</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr"/>
+      <c r="G312" t="inlineStr"/>
+      <c r="H312" t="inlineStr"/>
+      <c r="I312" t="inlineStr"/>
+      <c r="J312" t="inlineStr"/>
+      <c r="K312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>65562</v>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>2808 W Broadway</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.263883932125, 'Longitude': -123.168604373932}</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>2025-06-01T01:23:39.355Z</t>
+        </is>
+      </c>
+      <c r="G313" t="n">
+        <v>156.9</v>
+      </c>
+      <c r="H313" t="inlineStr">
+        <is>
+          <t>2025-05-31T20:01:03.497Z</t>
+        </is>
+      </c>
+      <c r="I313" t="n">
+        <v>182.9</v>
+      </c>
+      <c r="J313" t="inlineStr"/>
+      <c r="K313" t="inlineStr"/>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>113305</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>3596 W 41st Ave</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.234385296079, 'Longitude': -123.184762001038}</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>2025-05-31T23:56:16.495Z</t>
+        </is>
+      </c>
+      <c r="G314" t="n">
+        <v>160.9</v>
+      </c>
+      <c r="H314" t="inlineStr">
+        <is>
+          <t>2025-05-31T23:57:11.768Z</t>
+        </is>
+      </c>
+      <c r="I314" t="n">
+        <v>190.9</v>
+      </c>
+      <c r="J314" t="inlineStr"/>
+      <c r="K314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>65570</v>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>2103 W Broadway</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.264135981257, 'Longitude': -123.153326511383}</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>2025-06-01T14:48:37.518Z</t>
+        </is>
+      </c>
+      <c r="G315" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H315" t="inlineStr">
+        <is>
+          <t>2025-05-31T03:25:54.254Z</t>
+        </is>
+      </c>
+      <c r="I315" t="n">
+        <v>186.9</v>
+      </c>
+      <c r="J315" t="inlineStr"/>
+      <c r="K315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>65554</v>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>1795 W Broadway</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.264037962303, 'Longitude': -123.145408630371}</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:11:58.279Z</t>
+        </is>
+      </c>
+      <c r="G316" t="n">
+        <v>159.9</v>
+      </c>
+      <c r="H316" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:11:58.326Z</t>
+        </is>
+      </c>
+      <c r="I316" t="n">
+        <v>186.9</v>
+      </c>
+      <c r="J316" t="inlineStr"/>
+      <c r="K316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>65571</v>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>4314 W 10th Ave</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.263533861752, 'Longitude': -123.203430175781}</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>2025-05-31T16:36:48.315Z</t>
+        </is>
+      </c>
+      <c r="G317" t="n">
+        <v>160.9</v>
+      </c>
+      <c r="H317" t="inlineStr">
+        <is>
+          <t>2025-05-31T16:36:48.330Z</t>
+        </is>
+      </c>
+      <c r="I317" t="n">
+        <v>190.9</v>
+      </c>
+      <c r="J317" t="inlineStr"/>
+      <c r="K317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>65565</v>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>1896 W 4th Ave</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.267881559667, 'Longitude': -123.14772605896}</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:42:32.930Z</t>
+        </is>
+      </c>
+      <c r="G318" t="n">
+        <v>156.9</v>
+      </c>
+      <c r="H318" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:42:32.977Z</t>
+        </is>
+      </c>
+      <c r="I318" t="n">
+        <v>181.9</v>
+      </c>
+      <c r="J318" t="inlineStr"/>
+      <c r="K318" t="inlineStr"/>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>32376</v>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>1503 W 41st Ave</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.234634576953, 'Longitude': -123.139971792698}</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:39:04.127Z</t>
+        </is>
+      </c>
+      <c r="G319" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H319" t="inlineStr"/>
+      <c r="I319" t="inlineStr"/>
+      <c r="J319" t="inlineStr"/>
+      <c r="K319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>65549</v>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>5702 Granville St</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.234036184118, 'Longitude': -123.139244914055}</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:38:44.942Z</t>
+        </is>
+      </c>
+      <c r="G320" t="n">
+        <v>159.9</v>
+      </c>
+      <c r="H320" t="inlineStr"/>
+      <c r="I320" t="inlineStr"/>
+      <c r="J320" t="inlineStr"/>
+      <c r="K320" t="inlineStr"/>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>65543</v>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>1900 Burrard St</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2685375, 'Longitude': -123.1453067}</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:44:32.009Z</t>
+        </is>
+      </c>
+      <c r="G321" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H321" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:12:31.316Z</t>
+        </is>
+      </c>
+      <c r="I321" t="n">
+        <v>185.9</v>
+      </c>
+      <c r="J321" t="inlineStr"/>
+      <c r="K321" t="inlineStr"/>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>65563</v>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>1743 Burrard St</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.270429790667, 'Longitude': -123.145886063576}</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:47:41.336Z</t>
+        </is>
+      </c>
+      <c r="G322" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H322" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:12:23.017Z</t>
+        </is>
+      </c>
+      <c r="I322" t="n">
+        <v>181.9</v>
+      </c>
+      <c r="J322" t="inlineStr"/>
+      <c r="K322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>72747</v>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>1010 W King Edward Ave</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.249188, 'Longitude': -123.127767}</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:11:56.981Z</t>
+        </is>
+      </c>
+      <c r="G323" t="n">
+        <v>153.9</v>
+      </c>
+      <c r="H323" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:11:57.216Z</t>
+        </is>
+      </c>
+      <c r="I323" t="n">
+        <v>204.9</v>
+      </c>
+      <c r="J323" t="inlineStr"/>
+      <c r="K323" t="inlineStr"/>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>32375</v>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>4110 Oak St</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.24894071957, 'Longitude': -123.127040863037}</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>2025-06-01T06:38:02.410Z</t>
+        </is>
+      </c>
+      <c r="G324" t="n">
+        <v>146.9</v>
+      </c>
+      <c r="H324" t="inlineStr">
+        <is>
+          <t>2025-06-01T02:35:00.276Z</t>
+        </is>
+      </c>
+      <c r="I324" t="n">
+        <v>208.9</v>
+      </c>
+      <c r="J324" t="inlineStr"/>
+      <c r="K324" t="inlineStr"/>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>65564</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>5680 Oak St</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.234217162181, 'Longitude': -123.127684593201}</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:59:51.947Z</t>
+        </is>
+      </c>
+      <c r="G325" t="n">
+        <v>146.9</v>
+      </c>
+      <c r="H325" t="inlineStr">
+        <is>
+          <t>2025-06-01T13:34:26.116Z</t>
+        </is>
+      </c>
+      <c r="I325" t="n">
+        <v>171.9</v>
+      </c>
+      <c r="J325" t="inlineStr"/>
+      <c r="K325" t="inlineStr"/>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>32372</v>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>6525 Oak St</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.226226639452, 'Longitude': -123.128687739372}</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>2025-06-01T09:24:48.427Z</t>
+        </is>
+      </c>
+      <c r="G326" t="n">
+        <v>159.9</v>
+      </c>
+      <c r="H326" t="inlineStr"/>
+      <c r="I326" t="inlineStr"/>
+      <c r="J326" t="inlineStr"/>
+      <c r="K326" t="inlineStr"/>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>9707</v>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>1205 Burrard St</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.279145231489, 'Longitude': -123.12982365489}</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>2025-06-01T12:39:33.610Z</t>
+        </is>
+      </c>
+      <c r="G327" t="n">
+        <v>155.9</v>
+      </c>
+      <c r="H327" t="inlineStr">
+        <is>
+          <t>2025-06-01T01:39:50.050Z</t>
+        </is>
+      </c>
+      <c r="I327" t="n">
+        <v>200.9</v>
+      </c>
+      <c r="J327" t="inlineStr"/>
+      <c r="K327" t="inlineStr"/>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>65566</v>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>8072 Granville St</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.212495055855, 'Longitude': -123.14013004303}</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:35:51.923Z</t>
+        </is>
+      </c>
+      <c r="G328" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H328" t="inlineStr">
+        <is>
+          <t>2025-06-01T13:34:18.256Z</t>
+        </is>
+      </c>
+      <c r="I328" t="n">
+        <v>174.9</v>
+      </c>
+      <c r="J328" t="inlineStr"/>
+      <c r="K328" t="inlineStr"/>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>65572</v>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>8686 Granville St</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.207280329467, 'Longitude': -123.140280246735}</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:53:42</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>2025-05-31T07:05:25.815Z</t>
+        </is>
+      </c>
+      <c r="G329" t="n">
+        <v>176.9</v>
+      </c>
+      <c r="H329" t="inlineStr">
+        <is>
+          <t>2025-05-31T07:05:25.925Z</t>
+        </is>
+      </c>
+      <c r="I329" t="n">
+        <v>208.9</v>
+      </c>
+      <c r="J329" t="inlineStr"/>
+      <c r="K329" t="inlineStr"/>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>65558</v>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>1390 E 33rd Ave</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.240045470021, 'Longitude': -123.076765537262}</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>2025-06-01T06:59:55.504Z</t>
+        </is>
+      </c>
+      <c r="G330" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H330" t="inlineStr">
+        <is>
+          <t>2025-06-01T08:32:06.533Z</t>
+        </is>
+      </c>
+      <c r="I330" t="n">
+        <v>172.9</v>
+      </c>
+      <c r="J330" t="inlineStr"/>
+      <c r="K330" t="inlineStr"/>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>83394</v>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>4064 Fraser St</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.248864, 'Longitude': -123.09002}</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>2025-06-01T06:21:26.209Z</t>
+        </is>
+      </c>
+      <c r="G331" t="n">
+        <v>159.9</v>
+      </c>
+      <c r="H331" t="inlineStr"/>
+      <c r="I331" t="inlineStr"/>
+      <c r="J331" t="inlineStr"/>
+      <c r="K331" t="inlineStr"/>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>65573</v>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>1396 E 41st Ave</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.232593005895, 'Longitude': -123.07728856802}</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>2025-06-01T12:09:36.710Z</t>
+        </is>
+      </c>
+      <c r="G332" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H332" t="inlineStr">
+        <is>
+          <t>2025-05-31T09:55:02.588Z</t>
+        </is>
+      </c>
+      <c r="I332" t="n">
+        <v>190.9</v>
+      </c>
+      <c r="J332" t="inlineStr"/>
+      <c r="K332" t="inlineStr"/>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>80714</v>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Husky</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>4933 Victoria Dr</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2397388, 'Longitude': -123.065748}</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:54:00.470Z</t>
+        </is>
+      </c>
+      <c r="G333" t="n">
+        <v>156.9</v>
+      </c>
+      <c r="H333" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:19:58.451Z</t>
+        </is>
+      </c>
+      <c r="I333" t="n">
+        <v>181.9</v>
+      </c>
+      <c r="J333" t="inlineStr"/>
+      <c r="K333" t="inlineStr"/>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>65552</v>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>2001 Kingsway</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.245312771918, 'Longitude': -123.064910173416}</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:53:35.920Z</t>
+        </is>
+      </c>
+      <c r="G334" t="n">
+        <v>159.9</v>
+      </c>
+      <c r="H334" t="inlineStr"/>
+      <c r="I334" t="inlineStr"/>
+      <c r="J334" t="inlineStr"/>
+      <c r="K334" t="inlineStr"/>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>65538</v>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>5252 Victoria Dr</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2372145, 'Longitude': -123.0650857}</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:53:40.472Z</t>
+        </is>
+      </c>
+      <c r="G335" t="n">
+        <v>156.9</v>
+      </c>
+      <c r="H335" t="inlineStr">
+        <is>
+          <t>2025-05-31T18:02:26.415Z</t>
+        </is>
+      </c>
+      <c r="I335" t="n">
+        <v>191.9</v>
+      </c>
+      <c r="J335" t="inlineStr"/>
+      <c r="K335" t="inlineStr"/>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
+        <v>90814</v>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>2277 Kingsway</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.242132845692, 'Longitude': -123.058204650879}</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:19:51.107Z</t>
+        </is>
+      </c>
+      <c r="G336" t="n">
+        <v>150.9</v>
+      </c>
+      <c r="H336" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:19:51.188Z</t>
+        </is>
+      </c>
+      <c r="I336" t="n">
+        <v>175.9</v>
+      </c>
+      <c r="J336" t="inlineStr"/>
+      <c r="K336" t="inlineStr"/>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
+        <v>39768</v>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>5736 Main St</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2325708, 'Longitude': -123.1010069}</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F337" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:29:08.825Z</t>
+        </is>
+      </c>
+      <c r="G337" t="n">
+        <v>151.9</v>
+      </c>
+      <c r="H337" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:12:17.857Z</t>
+        </is>
+      </c>
+      <c r="I337" t="n">
+        <v>177.9</v>
+      </c>
+      <c r="J337" t="inlineStr"/>
+      <c r="K337" t="inlineStr"/>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>9710</v>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>1295 E 12th Ave</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.259878978744, 'Longitude': -123.078074455261}</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F338" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:14:51.193Z</t>
+        </is>
+      </c>
+      <c r="G338" t="n">
+        <v>143.9</v>
+      </c>
+      <c r="H338" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:21:09.237Z</t>
+        </is>
+      </c>
+      <c r="I338" t="n">
+        <v>188.9</v>
+      </c>
+      <c r="J338" t="inlineStr"/>
+      <c r="K338" t="inlineStr"/>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>99146</v>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Super Save Gas</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>1317 E 12th Ave</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.259758544957, 'Longitude': -123.077272474766}</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:14:42.090Z</t>
+        </is>
+      </c>
+      <c r="G339" t="n">
+        <v>143.9</v>
+      </c>
+      <c r="H339" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:20:06.615Z</t>
+        </is>
+      </c>
+      <c r="I339" t="n">
+        <v>176.9</v>
+      </c>
+      <c r="J339" t="inlineStr"/>
+      <c r="K339" t="inlineStr"/>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>65560</v>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>1289 E Broadway</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.262693682723, 'Longitude': -123.078117370605}</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F340" t="inlineStr">
+        <is>
+          <t>2025-06-01T08:30:06.167Z</t>
+        </is>
+      </c>
+      <c r="G340" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H340" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:14:23.876Z</t>
+        </is>
+      </c>
+      <c r="I340" t="n">
+        <v>199.9</v>
+      </c>
+      <c r="J340" t="inlineStr"/>
+      <c r="K340" t="inlineStr"/>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>65557</v>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>2120 Grandview Hwy S</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2591601, 'Longitude': -123.0617495}</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>2025-06-01T08:31:50.639Z</t>
+        </is>
+      </c>
+      <c r="G341" t="n">
+        <v>150.9</v>
+      </c>
+      <c r="H341" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:19:24.708Z</t>
+        </is>
+      </c>
+      <c r="I341" t="n">
+        <v>191.9</v>
+      </c>
+      <c r="J341" t="inlineStr"/>
+      <c r="K341" t="inlineStr"/>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>71502</v>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>2748 Main St</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2604441, 'Longitude': -123.1005869}</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F342" t="inlineStr">
+        <is>
+          <t>2025-06-01T08:27:47.662Z</t>
+        </is>
+      </c>
+      <c r="G342" t="n">
+        <v>151.9</v>
+      </c>
+      <c r="H342" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:15:28.765Z</t>
+        </is>
+      </c>
+      <c r="I342" t="n">
+        <v>177.9</v>
+      </c>
+      <c r="J342" t="inlineStr"/>
+      <c r="K342" t="inlineStr"/>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>65559</v>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>6502 Victoria Dr</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.224996944057, 'Longitude': -123.065521717072}</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F343" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:43:07.963Z</t>
+        </is>
+      </c>
+      <c r="G343" t="n">
+        <v>156.9</v>
+      </c>
+      <c r="H343" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:20:11.563Z</t>
+        </is>
+      </c>
+      <c r="I343" t="n">
+        <v>181.9</v>
+      </c>
+      <c r="J343" t="inlineStr"/>
+      <c r="K343" t="inlineStr"/>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>89943</v>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>6808 Victoria Dr</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2220242, 'Longitude': -123.0654247}</t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F344" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:45:52.270Z</t>
+        </is>
+      </c>
+      <c r="G344" t="n">
+        <v>156.9</v>
+      </c>
+      <c r="H344" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:45:52.301Z</t>
+        </is>
+      </c>
+      <c r="I344" t="n">
+        <v>182.9</v>
+      </c>
+      <c r="J344" t="inlineStr"/>
+      <c r="K344" t="inlineStr"/>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>86880</v>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>7282 Knight St</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.218250007984, 'Longitude': -123.076816499233}</t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F345" t="inlineStr">
+        <is>
+          <t>2025-06-01T10:01:43.769Z</t>
+        </is>
+      </c>
+      <c r="G345" t="n">
+        <v>156.9</v>
+      </c>
+      <c r="H345" t="inlineStr">
+        <is>
+          <t>2025-06-01T06:49:00.026Z</t>
+        </is>
+      </c>
+      <c r="I345" t="n">
+        <v>192.9</v>
+      </c>
+      <c r="J345" t="inlineStr"/>
+      <c r="K345" t="inlineStr"/>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>65537</v>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>2918 Kingsway</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.23608, 'Longitude': -123.0454858}</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F346" t="inlineStr">
+        <is>
+          <t>2025-06-01T08:44:31.473Z</t>
+        </is>
+      </c>
+      <c r="G346" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H346" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:20:41.437Z</t>
+        </is>
+      </c>
+      <c r="I346" t="n">
+        <v>186.9</v>
+      </c>
+      <c r="J346" t="inlineStr"/>
+      <c r="K346" t="inlineStr"/>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
+        <v>65536</v>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>7309 Knight St</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2177761, 'Longitude': -123.0775405}</t>
+        </is>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F347" t="inlineStr">
+        <is>
+          <t>2025-06-01T10:49:47.608Z</t>
+        </is>
+      </c>
+      <c r="G347" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H347" t="inlineStr">
+        <is>
+          <t>2025-06-01T06:49:13.464Z</t>
+        </is>
+      </c>
+      <c r="I347" t="n">
+        <v>200.9</v>
+      </c>
+      <c r="J347" t="inlineStr"/>
+      <c r="K347" t="inlineStr"/>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
+        <v>65535</v>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>2605 E 49th Ave</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2251291, 'Longitude': -123.0545048}</t>
+        </is>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F348" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:47:56.888Z</t>
+        </is>
+      </c>
+      <c r="G348" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H348" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:47:56.950Z</t>
+        </is>
+      </c>
+      <c r="I348" t="n">
+        <v>187.9</v>
+      </c>
+      <c r="J348" t="inlineStr"/>
+      <c r="K348" t="inlineStr"/>
+    </row>
+    <row r="349">
+      <c r="A349" t="n">
+        <v>65539</v>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>2902 Grandview Hwy</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2579053, 'Longitude': -123.0438464}</t>
+        </is>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:56:35</t>
+        </is>
+      </c>
+      <c r="F349" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:15:39.400Z</t>
+        </is>
+      </c>
+      <c r="G349" t="n">
+        <v>150.9</v>
+      </c>
+      <c r="H349" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:15:39.462Z</t>
+        </is>
+      </c>
+      <c r="I349" t="n">
+        <v>191.9</v>
+      </c>
+      <c r="J349" t="inlineStr"/>
+      <c r="K349" t="inlineStr"/>
+    </row>
+    <row r="350">
+      <c r="A350" t="n">
+        <v>77015</v>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Super Save Gas</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>6000 No 5 Rd</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.169873456637, 'Longitude': -123.091178619746}</t>
+        </is>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F350" t="inlineStr">
+        <is>
+          <t>2025-06-01T04:23:21.131Z</t>
+        </is>
+      </c>
+      <c r="G350" t="n">
+        <v>146.9</v>
+      </c>
+      <c r="H350" t="inlineStr">
+        <is>
+          <t>2025-06-01T13:33:21.366Z</t>
+        </is>
+      </c>
+      <c r="I350" t="n">
+        <v>171.9</v>
+      </c>
+      <c r="J350" t="inlineStr"/>
+      <c r="K350" t="inlineStr"/>
+    </row>
+    <row r="351">
+      <c r="A351" t="n">
+        <v>65511</v>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12011 Bridgeport Rd</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1923857, 'Longitude': -123.0911072}</t>
+        </is>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F351" t="inlineStr">
+        <is>
+          <t>2025-06-01T14:12:40.071Z</t>
+        </is>
+      </c>
+      <c r="G351" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H351" t="inlineStr">
+        <is>
+          <t>2025-06-01T08:39:35.945Z</t>
+        </is>
+      </c>
+      <c r="I351" t="n">
+        <v>183.9</v>
+      </c>
+      <c r="J351" t="inlineStr"/>
+      <c r="K351" t="inlineStr"/>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>86650</v>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>9100 Westminster Hwy</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.169856952787, 'Longitude': -123.123961687088}</t>
+        </is>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F352" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:48:13.960Z</t>
+        </is>
+      </c>
+      <c r="G352" t="n">
+        <v>146.9</v>
+      </c>
+      <c r="H352" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:57:30.357Z</t>
+        </is>
+      </c>
+      <c r="I352" t="n">
+        <v>179.9</v>
+      </c>
+      <c r="J352" t="inlineStr"/>
+      <c r="K352" t="inlineStr"/>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
+        <v>77218</v>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>5511 Garden City Rd</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.173339635958, 'Longitude': -123.124954104424}</t>
+        </is>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F353" t="inlineStr">
+        <is>
+          <t>2025-06-01T08:29:51.093Z</t>
+        </is>
+      </c>
+      <c r="G353" t="n">
+        <v>145.9</v>
+      </c>
+      <c r="H353" t="inlineStr">
+        <is>
+          <t>2025-06-01T01:47:40.302Z</t>
+        </is>
+      </c>
+      <c r="I353" t="n">
+        <v>200.9</v>
+      </c>
+      <c r="J353" t="inlineStr"/>
+      <c r="K353" t="inlineStr"/>
+    </row>
+    <row r="354">
+      <c r="A354" t="n">
+        <v>77228</v>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>9100 Cambie Rd</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1843249, 'Longitude': -123.1236078}</t>
+        </is>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F354" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:07:32.704Z</t>
+        </is>
+      </c>
+      <c r="G354" t="n">
+        <v>145.9</v>
+      </c>
+      <c r="H354" t="inlineStr">
+        <is>
+          <t>2025-05-31T23:49:46.480Z</t>
+        </is>
+      </c>
+      <c r="I354" t="n">
+        <v>181.9</v>
+      </c>
+      <c r="J354" t="inlineStr"/>
+      <c r="K354" t="inlineStr"/>
+    </row>
+    <row r="355">
+      <c r="A355" t="n">
+        <v>83384</v>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>9060 Bridgeport Rd</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.192001, 'Longitude': -123.124004}</t>
+        </is>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F355" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:24:07.338Z</t>
+        </is>
+      </c>
+      <c r="G355" t="n">
+        <v>148.9</v>
+      </c>
+      <c r="H355" t="inlineStr">
+        <is>
+          <t>2025-06-01T04:44:26.424Z</t>
+        </is>
+      </c>
+      <c r="I355" t="n">
+        <v>189.9</v>
+      </c>
+      <c r="J355" t="inlineStr"/>
+      <c r="K355" t="inlineStr"/>
+    </row>
+    <row r="356">
+      <c r="A356" t="n">
+        <v>77202</v>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>8151 Granville Ave</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.162989071149, 'Longitude': -123.134229183197}</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>2025-06-01T06:36:56.417Z</t>
+        </is>
+      </c>
+      <c r="G356" t="n">
+        <v>144.9</v>
+      </c>
+      <c r="H356" t="inlineStr">
+        <is>
+          <t>2025-06-01T13:33:32.437Z</t>
+        </is>
+      </c>
+      <c r="I356" t="n">
+        <v>173.9</v>
+      </c>
+      <c r="J356" t="inlineStr"/>
+      <c r="K356" t="inlineStr"/>
+    </row>
+    <row r="357">
+      <c r="A357" t="n">
+        <v>77243</v>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Mobil</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>4651 No  3 Rd</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.179182137142, 'Longitude': -123.137152791023}</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F357" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:08:26.913Z</t>
+        </is>
+      </c>
+      <c r="G357" t="n">
+        <v>148.9</v>
+      </c>
+      <c r="H357" t="inlineStr">
+        <is>
+          <t>2025-06-01T06:33:33.347Z</t>
+        </is>
+      </c>
+      <c r="I357" t="n">
+        <v>173.9</v>
+      </c>
+      <c r="J357" t="inlineStr"/>
+      <c r="K357" t="inlineStr"/>
+    </row>
+    <row r="358">
+      <c r="A358" t="n">
+        <v>83387</v>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>710 SE Marine Dr</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.21081995506, 'Longitude': -123.090755939484}</t>
+        </is>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F358" t="inlineStr">
+        <is>
+          <t>2025-06-01T06:54:00.199Z</t>
+        </is>
+      </c>
+      <c r="G358" t="n">
+        <v>149.9</v>
+      </c>
+      <c r="H358" t="inlineStr">
+        <is>
+          <t>2025-06-01T02:52:14.151Z</t>
+        </is>
+      </c>
+      <c r="I358" t="n">
+        <v>178.9</v>
+      </c>
+      <c r="J358" t="inlineStr"/>
+      <c r="K358" t="inlineStr"/>
+    </row>
+    <row r="359">
+      <c r="A359" t="n">
+        <v>65551</v>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>688 SE Marine Dr</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.210798928329, 'Longitude': -123.09152841568}</t>
+        </is>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F359" t="inlineStr">
+        <is>
+          <t>2025-06-01T08:23:17.734Z</t>
+        </is>
+      </c>
+      <c r="G359" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="H359" t="inlineStr">
+        <is>
+          <t>2025-05-31T22:41:12.850Z</t>
+        </is>
+      </c>
+      <c r="I359" t="n">
+        <v>189.9</v>
+      </c>
+      <c r="J359" t="inlineStr"/>
+      <c r="K359" t="inlineStr"/>
+    </row>
+    <row r="360">
+      <c r="A360" t="n">
+        <v>77235</v>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Domo</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4071 No 3 Rd </t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.18409178594, 'Longitude': -123.136823830688}</t>
+        </is>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F360" t="inlineStr">
+        <is>
+          <t>2025-06-01T02:59:56.911Z</t>
+        </is>
+      </c>
+      <c r="G360" t="n">
+        <v>148.9</v>
+      </c>
+      <c r="H360" t="inlineStr">
+        <is>
+          <t>2025-06-01T13:33:41.808Z</t>
+        </is>
+      </c>
+      <c r="I360" t="n">
+        <v>173.9</v>
+      </c>
+      <c r="J360" t="inlineStr"/>
+      <c r="K360" t="inlineStr"/>
+    </row>
+    <row r="361">
+      <c r="A361" t="n">
+        <v>82925</v>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Mobil</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>350 SE Marine Dr</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.210245, 'Longitude': -123.099328}</t>
+        </is>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F361" t="inlineStr">
+        <is>
+          <t>2025-06-01T04:38:22.123Z</t>
+        </is>
+      </c>
+      <c r="G361" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="H361" t="inlineStr">
+        <is>
+          <t>2025-05-31T22:41:36.541Z</t>
+        </is>
+      </c>
+      <c r="I361" t="n">
+        <v>191.9</v>
+      </c>
+      <c r="J361" t="inlineStr"/>
+      <c r="K361" t="inlineStr"/>
+    </row>
+    <row r="362">
+      <c r="A362" t="n">
+        <v>109205</v>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>11991 Steveston Hwy</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.133556536531, 'Longitude': -123.092424273491}</t>
+        </is>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F362" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:31:31.114Z</t>
+        </is>
+      </c>
+      <c r="G362" t="n">
+        <v>145.9</v>
+      </c>
+      <c r="H362" t="inlineStr">
+        <is>
+          <t>2025-06-01T13:33:11.500Z</t>
+        </is>
+      </c>
+      <c r="I362" t="n">
+        <v>179.9</v>
+      </c>
+      <c r="J362" t="inlineStr"/>
+      <c r="K362" t="inlineStr"/>
+    </row>
+    <row r="363">
+      <c r="A363" t="n">
+        <v>65540</v>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>196 SE Marine Dr</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2106867, 'Longitude': -123.1027436}</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F363" t="inlineStr">
+        <is>
+          <t>2025-06-01T11:42:57.059Z</t>
+        </is>
+      </c>
+      <c r="G363" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="H363" t="inlineStr">
+        <is>
+          <t>2025-05-31T22:41:59.850Z</t>
+        </is>
+      </c>
+      <c r="I363" t="n">
+        <v>192.7</v>
+      </c>
+      <c r="J363" t="inlineStr"/>
+      <c r="K363" t="inlineStr"/>
+    </row>
+    <row r="364">
+      <c r="A364" t="n">
+        <v>65512</v>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>11131 No 5 Rd</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1328393, 'Longitude': -123.0926312}</t>
+        </is>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:48:20.195Z</t>
+        </is>
+      </c>
+      <c r="G364" t="n">
+        <v>145.9</v>
+      </c>
+      <c r="H364" t="inlineStr">
+        <is>
+          <t>2025-06-01T12:14:35.750Z</t>
+        </is>
+      </c>
+      <c r="I364" t="n">
+        <v>204.9</v>
+      </c>
+      <c r="J364" t="inlineStr"/>
+      <c r="K364" t="inlineStr"/>
+    </row>
+    <row r="365">
+      <c r="A365" t="n">
+        <v>77205</v>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7951 No 3 Rd </t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1558882, 'Longitude': -123.1369625}</t>
+        </is>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F365" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:01:37.299Z</t>
+        </is>
+      </c>
+      <c r="G365" t="n">
+        <v>145.9</v>
+      </c>
+      <c r="H365" t="inlineStr">
+        <is>
+          <t>2025-06-01T00:58:26.467Z</t>
+        </is>
+      </c>
+      <c r="I365" t="n">
+        <v>194.9</v>
+      </c>
+      <c r="J365" t="inlineStr"/>
+      <c r="K365" t="inlineStr"/>
+    </row>
+    <row r="366">
+      <c r="A366" t="n">
+        <v>65536</v>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>7309 Knight St</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2177761, 'Longitude': -123.0775405}</t>
+        </is>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F366" t="inlineStr">
+        <is>
+          <t>2025-06-01T10:49:47.608Z</t>
+        </is>
+      </c>
+      <c r="G366" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H366" t="inlineStr">
+        <is>
+          <t>2025-06-01T06:49:13.464Z</t>
+        </is>
+      </c>
+      <c r="I366" t="n">
+        <v>200.9</v>
+      </c>
+      <c r="J366" t="inlineStr"/>
+      <c r="K366" t="inlineStr"/>
+    </row>
+    <row r="367">
+      <c r="A367" t="n">
+        <v>86880</v>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>7282 Knight St</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.218250007984, 'Longitude': -123.076816499233}</t>
+        </is>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F367" t="inlineStr">
+        <is>
+          <t>2025-06-01T10:01:43.769Z</t>
+        </is>
+      </c>
+      <c r="G367" t="n">
+        <v>156.9</v>
+      </c>
+      <c r="H367" t="inlineStr">
+        <is>
+          <t>2025-06-01T06:49:00.026Z</t>
+        </is>
+      </c>
+      <c r="I367" t="n">
+        <v>192.9</v>
+      </c>
+      <c r="J367" t="inlineStr"/>
+      <c r="K367" t="inlineStr"/>
+    </row>
+    <row r="368">
+      <c r="A368" t="n">
+        <v>65556</v>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>709 SW Marine Dr</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.20806537721, 'Longitude': -123.123285770416}</t>
+        </is>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F368" t="inlineStr">
+        <is>
+          <t>2025-06-01T12:30:47.378Z</t>
+        </is>
+      </c>
+      <c r="G368" t="n">
+        <v>152.9</v>
+      </c>
+      <c r="H368" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:12:03.073Z</t>
+        </is>
+      </c>
+      <c r="I368" t="n">
+        <v>184.9</v>
+      </c>
+      <c r="J368" t="inlineStr"/>
+      <c r="K368" t="inlineStr"/>
+    </row>
+    <row r="369">
+      <c r="A369" t="n">
+        <v>86937</v>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>8655 Boundary Rd</t>
+        </is>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.20476, 'Longitude': -123.02398}</t>
+        </is>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>2025-06-01 22:59:26</t>
+        </is>
+      </c>
+      <c r="F369" t="inlineStr">
+        <is>
+          <t>2025-06-01T14:35:32.859Z</t>
+        </is>
+      </c>
+      <c r="G369" t="n">
+        <v>156.9</v>
+      </c>
+      <c r="H369" t="inlineStr">
+        <is>
+          <t>2025-06-01T14:35:32.891Z</t>
+        </is>
+      </c>
+      <c r="I369" t="n">
+        <v>202.9</v>
+      </c>
+      <c r="J369" t="inlineStr"/>
+      <c r="K369" t="inlineStr"/>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>65515</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>4011 Francis Rd</t>
+        </is>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.14867500071, 'Longitude': -123.180856704712}</t>
+        </is>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F370" t="inlineStr">
+        <is>
+          <t>2025-06-01T04:41:32.090Z</t>
+        </is>
+      </c>
+      <c r="G370" t="n">
+        <v>146.9</v>
+      </c>
+      <c r="H370" t="inlineStr">
+        <is>
+          <t>2025-06-01T11:27:10.927Z</t>
+        </is>
+      </c>
+      <c r="I370" t="n">
+        <v>202.9</v>
+      </c>
+      <c r="J370" t="inlineStr"/>
+      <c r="K370" t="inlineStr"/>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>77205</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7951 No 3 Rd </t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1558882, 'Longitude': -123.1369625}</t>
+        </is>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F371" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:01:37.299Z</t>
+        </is>
+      </c>
+      <c r="G371" t="n">
+        <v>145.9</v>
+      </c>
+      <c r="H371" t="inlineStr">
+        <is>
+          <t>2025-06-01T00:58:26.467Z</t>
+        </is>
+      </c>
+      <c r="I371" t="n">
+        <v>194.9</v>
+      </c>
+      <c r="J371" t="inlineStr"/>
+      <c r="K371" t="inlineStr"/>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>77223</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>7991 No 1 Rd</t>
+        </is>
+      </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.155888686563, 'Longitude': -123.181414604187}</t>
+        </is>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F372" t="inlineStr">
+        <is>
+          <t>2025-06-01T11:25:38.309Z</t>
+        </is>
+      </c>
+      <c r="G372" t="n">
+        <v>146.9</v>
+      </c>
+      <c r="H372" t="inlineStr">
+        <is>
+          <t>2025-06-01T11:26:04.566Z</t>
+        </is>
+      </c>
+      <c r="I372" t="n">
+        <v>191.9</v>
+      </c>
+      <c r="J372" t="inlineStr"/>
+      <c r="K372" t="inlineStr"/>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>65514</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>7980 Williams Rd</t>
+        </is>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.140582914547, 'Longitude': -123.137168884277}</t>
+        </is>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F373" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:02:22.809Z</t>
+        </is>
+      </c>
+      <c r="G373" t="n">
+        <v>145.9</v>
+      </c>
+      <c r="H373" t="inlineStr">
+        <is>
+          <t>2025-06-01T13:33:26.527Z</t>
+        </is>
+      </c>
+      <c r="I373" t="n">
+        <v>170.9</v>
+      </c>
+      <c r="J373" t="inlineStr"/>
+      <c r="K373" t="inlineStr"/>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>77232</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5900 Westminster Hwy </t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1698419, 'Longitude': -123.159282}</t>
+        </is>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F374" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:08:41.958Z</t>
+        </is>
+      </c>
+      <c r="G374" t="n">
+        <v>145.9</v>
+      </c>
+      <c r="H374" t="inlineStr">
+        <is>
+          <t>2025-06-01T13:33:47.561Z</t>
+        </is>
+      </c>
+      <c r="I374" t="n">
+        <v>171.9</v>
+      </c>
+      <c r="J374" t="inlineStr"/>
+      <c r="K374" t="inlineStr"/>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>77202</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>8151 Granville Ave</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.162989071149, 'Longitude': -123.134229183197}</t>
+        </is>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F375" t="inlineStr">
+        <is>
+          <t>2025-06-01T06:36:56.417Z</t>
+        </is>
+      </c>
+      <c r="G375" t="n">
+        <v>144.9</v>
+      </c>
+      <c r="H375" t="inlineStr">
+        <is>
+          <t>2025-06-01T13:33:32.437Z</t>
+        </is>
+      </c>
+      <c r="I375" t="n">
+        <v>173.9</v>
+      </c>
+      <c r="J375" t="inlineStr"/>
+      <c r="K375" t="inlineStr"/>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>86650</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>9100 Westminster Hwy</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.169856952787, 'Longitude': -123.123961687088}</t>
+        </is>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F376" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:48:13.960Z</t>
+        </is>
+      </c>
+      <c r="G376" t="n">
+        <v>146.9</v>
+      </c>
+      <c r="H376" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:57:30.357Z</t>
+        </is>
+      </c>
+      <c r="I376" t="n">
+        <v>179.9</v>
+      </c>
+      <c r="J376" t="inlineStr"/>
+      <c r="K376" t="inlineStr"/>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>77218</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>5511 Garden City Rd</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.173339635958, 'Longitude': -123.124954104424}</t>
+        </is>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F377" t="inlineStr">
+        <is>
+          <t>2025-06-01T08:29:51.093Z</t>
+        </is>
+      </c>
+      <c r="G377" t="n">
+        <v>145.9</v>
+      </c>
+      <c r="H377" t="inlineStr">
+        <is>
+          <t>2025-06-01T01:47:40.302Z</t>
+        </is>
+      </c>
+      <c r="I377" t="n">
+        <v>200.9</v>
+      </c>
+      <c r="J377" t="inlineStr"/>
+      <c r="K377" t="inlineStr"/>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>77243</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Mobil</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>4651 No  3 Rd</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.179182137142, 'Longitude': -123.137152791023}</t>
+        </is>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F378" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:08:26.913Z</t>
+        </is>
+      </c>
+      <c r="G378" t="n">
+        <v>148.9</v>
+      </c>
+      <c r="H378" t="inlineStr">
+        <is>
+          <t>2025-06-01T06:33:33.347Z</t>
+        </is>
+      </c>
+      <c r="I378" t="n">
+        <v>173.9</v>
+      </c>
+      <c r="J378" t="inlineStr"/>
+      <c r="K378" t="inlineStr"/>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>77235</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Domo</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4071 No 3 Rd </t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.18409178594, 'Longitude': -123.136823830688}</t>
+        </is>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F379" t="inlineStr">
+        <is>
+          <t>2025-06-01T02:59:56.911Z</t>
+        </is>
+      </c>
+      <c r="G379" t="n">
+        <v>148.9</v>
+      </c>
+      <c r="H379" t="inlineStr">
+        <is>
+          <t>2025-06-01T13:33:41.808Z</t>
+        </is>
+      </c>
+      <c r="I379" t="n">
+        <v>173.9</v>
+      </c>
+      <c r="J379" t="inlineStr"/>
+      <c r="K379" t="inlineStr"/>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>77228</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>9100 Cambie Rd</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1843249, 'Longitude': -123.1236078}</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F380" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:07:32.704Z</t>
+        </is>
+      </c>
+      <c r="G380" t="n">
+        <v>145.9</v>
+      </c>
+      <c r="H380" t="inlineStr">
+        <is>
+          <t>2025-05-31T23:49:46.480Z</t>
+        </is>
+      </c>
+      <c r="I380" t="n">
+        <v>181.9</v>
+      </c>
+      <c r="J380" t="inlineStr"/>
+      <c r="K380" t="inlineStr"/>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>69163</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>5111 Grant McConachie Way</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.192919, 'Longitude': -123.166797}</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F381" t="inlineStr">
+        <is>
+          <t>2025-06-01T13:40:51.486Z</t>
+        </is>
+      </c>
+      <c r="G381" t="n">
+        <v>162.9</v>
+      </c>
+      <c r="H381" t="inlineStr">
+        <is>
+          <t>2025-06-01T00:05:13.562Z</t>
+        </is>
+      </c>
+      <c r="I381" t="n">
+        <v>176.9</v>
+      </c>
+      <c r="J381" t="inlineStr"/>
+      <c r="K381" t="inlineStr"/>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>109205</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Petro-Canada</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>11991 Steveston Hwy</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.133556536531, 'Longitude': -123.092424273491}</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F382" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:31:31.114Z</t>
+        </is>
+      </c>
+      <c r="G382" t="n">
+        <v>145.9</v>
+      </c>
+      <c r="H382" t="inlineStr">
+        <is>
+          <t>2025-06-01T13:33:11.500Z</t>
+        </is>
+      </c>
+      <c r="I382" t="n">
+        <v>179.9</v>
+      </c>
+      <c r="J382" t="inlineStr"/>
+      <c r="K382" t="inlineStr"/>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>65512</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>11131 No 5 Rd</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1328393, 'Longitude': -123.0926312}</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F383" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:48:20.195Z</t>
+        </is>
+      </c>
+      <c r="G383" t="n">
+        <v>145.9</v>
+      </c>
+      <c r="H383" t="inlineStr">
+        <is>
+          <t>2025-06-01T12:14:35.750Z</t>
+        </is>
+      </c>
+      <c r="I383" t="n">
+        <v>204.9</v>
+      </c>
+      <c r="J383" t="inlineStr"/>
+      <c r="K383" t="inlineStr"/>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>83384</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>9060 Bridgeport Rd</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.192001, 'Longitude': -123.124004}</t>
+        </is>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F384" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:24:07.338Z</t>
+        </is>
+      </c>
+      <c r="G384" t="n">
+        <v>148.9</v>
+      </c>
+      <c r="H384" t="inlineStr">
+        <is>
+          <t>2025-06-01T04:44:26.424Z</t>
+        </is>
+      </c>
+      <c r="I384" t="n">
+        <v>189.9</v>
+      </c>
+      <c r="J384" t="inlineStr"/>
+      <c r="K384" t="inlineStr"/>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>77015</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Super Save Gas</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>6000 No 5 Rd</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.169873456637, 'Longitude': -123.091178619746}</t>
+        </is>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F385" t="inlineStr">
+        <is>
+          <t>2025-06-01T04:23:21.131Z</t>
+        </is>
+      </c>
+      <c r="G385" t="n">
+        <v>146.9</v>
+      </c>
+      <c r="H385" t="inlineStr">
+        <is>
+          <t>2025-06-01T13:33:21.366Z</t>
+        </is>
+      </c>
+      <c r="I385" t="n">
+        <v>171.9</v>
+      </c>
+      <c r="J385" t="inlineStr"/>
+      <c r="K385" t="inlineStr"/>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>107728</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>8884 Granville St</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.2054215, 'Longitude': -123.1401677}</t>
+        </is>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F386" t="inlineStr">
+        <is>
+          <t>2025-06-01T07:55:53.680Z</t>
+        </is>
+      </c>
+      <c r="G386" t="n">
+        <v>147.9</v>
+      </c>
+      <c r="H386" t="inlineStr">
+        <is>
+          <t>2025-06-01T08:31:35.181Z</t>
+        </is>
+      </c>
+      <c r="I386" t="n">
+        <v>173.9</v>
+      </c>
+      <c r="J386" t="inlineStr"/>
+      <c r="K386" t="inlineStr"/>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>65572</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Shell</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>8686 Granville St</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.207280329467, 'Longitude': -123.140280246735}</t>
+        </is>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F387" t="inlineStr">
+        <is>
+          <t>2025-05-31T07:05:25.815Z</t>
+        </is>
+      </c>
+      <c r="G387" t="n">
+        <v>176.9</v>
+      </c>
+      <c r="H387" t="inlineStr">
+        <is>
+          <t>2025-05-31T07:05:25.925Z</t>
+        </is>
+      </c>
+      <c r="I387" t="n">
+        <v>208.9</v>
+      </c>
+      <c r="J387" t="inlineStr"/>
+      <c r="K387" t="inlineStr"/>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>65511</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Chevron</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12011 Bridgeport Rd</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.1923857, 'Longitude': -123.0911072}</t>
+        </is>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F388" t="inlineStr">
+        <is>
+          <t>2025-06-01T14:12:40.071Z</t>
+        </is>
+      </c>
+      <c r="G388" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="H388" t="inlineStr">
+        <is>
+          <t>2025-06-01T08:39:35.945Z</t>
+        </is>
+      </c>
+      <c r="I388" t="n">
+        <v>183.9</v>
+      </c>
+      <c r="J388" t="inlineStr"/>
+      <c r="K388" t="inlineStr"/>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>65556</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Esso</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>709 SW Marine Dr</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>{'Latitude': 49.20806537721, 'Longitude': -123.123285770416}</t>
+        </is>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>2025-06-01 23:02:17</t>
+        </is>
+      </c>
+      <c r="F389" t="inlineStr">
+        <is>
+          <t>2025-06-01T12:30:47.378Z</t>
+        </is>
+      </c>
+      <c r="G389" t="n">
+        <v>152.9</v>
+      </c>
+      <c r="H389" t="inlineStr">
+        <is>
+          <t>2025-06-01T05:12:03.073Z</t>
+        </is>
+      </c>
+      <c r="I389" t="n">
+        <v>184.9</v>
+      </c>
+      <c r="J389" t="inlineStr"/>
+      <c r="K389" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>